<commit_message>
updated audit and enabled tooltip on piecharts
</commit_message>
<xml_diff>
--- a/docs/HCD/508_Compliance_Audit.xlsx
+++ b/docs/HCD/508_Compliance_Audit.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhazelbaker\Desktop\Proposals\GSA BPA Agile RFQ\doc\HCD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27920" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
   <si>
     <t>508 STANDARD</t>
   </si>
@@ -522,12 +520,6 @@
     <t>ADS-Dev Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Fail - Chart is the only element that is non text. It does not contain alt or longdesc text. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fail -- Description does not exist. </t>
-  </si>
-  <si>
     <t xml:space="preserve">N/A as of now. A background image is in the works. </t>
   </si>
   <si>
@@ -540,9 +532,6 @@
     <t xml:space="preserve">Color is used for styling purposes only. The chart does use color to denote the event but it’s the sole item in the key. </t>
   </si>
   <si>
-    <t xml:space="preserve">Fail - App functionality is present when stylesheet is removed. Enhancement -- The chart labels intersect when stylesheets are removed. The percentage and symptom labels are not readable. Remainder of app content is readable and maintains the same order as the application. </t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -552,9 +541,6 @@
     <t xml:space="preserve">N/A -- Tables are not used for layout. </t>
   </si>
   <si>
-    <t xml:space="preserve">Fail -- Solve by adding scope="col" as an attribute for the table headers. See http://webaim.org/techniques/tables/data for more information. </t>
-  </si>
-  <si>
     <t xml:space="preserve">N/A -- Frames not present. </t>
   </si>
   <si>
@@ -570,9 +556,6 @@
     <t>Applets or plugins are not required</t>
   </si>
   <si>
-    <t xml:space="preserve">Fail - drug input form fields, remove drug button, nor the symptom dropdown contain descriptive form elements. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Scripting of these elements does not interfere with assistive technologies once brought into compliance. </t>
   </si>
   <si>
@@ -589,13 +572,34 @@
   </si>
   <si>
     <t>FAIL Criteria</t>
+  </si>
+  <si>
+    <t>Mouse over tool tips have been added to bar chart and pie charts</t>
+  </si>
+  <si>
+    <t>tooltips provied data</t>
+  </si>
+  <si>
+    <t>page describes the graphs/charts</t>
+  </si>
+  <si>
+    <t>Functionality partially works.</t>
+  </si>
+  <si>
+    <t>scope="col" has been added</t>
+  </si>
+  <si>
+    <t>Titles and descriptions exist</t>
+  </si>
+  <si>
+    <t>alternate text exists</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -643,8 +647,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,6 +668,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFAFAFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,7 +707,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -703,9 +718,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -713,6 +725,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -777,7 +795,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -812,7 +830,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -989,7 +1007,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -999,48 +1017,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="54.54296875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="36.81640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="34.54296875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="45" style="7" customWidth="1"/>
-    <col min="5" max="14" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="54.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="34.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="45" style="6" customWidth="1"/>
+    <col min="5" max="14" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="72.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+      <c r="D2" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="75">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1048,11 +1066,11 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="D3" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="90">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -1060,11 +1078,11 @@
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="D4" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -1072,11 +1090,11 @@
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+      <c r="D5" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="90">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -1084,11 +1102,11 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="D6" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -1096,24 +1114,24 @@
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1"/>
+    <row r="9" spans="1:4" ht="15" customHeight="1"/>
+    <row r="10" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="45">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1123,11 +1141,11 @@
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>18</v>
@@ -1135,24 +1153,24 @@
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="D12" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1"/>
+    <row r="14" spans="1:4" ht="15" customHeight="1"/>
+    <row r="15" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="45">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1162,11 +1180,11 @@
       <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -1174,24 +1192,24 @@
       <c r="C17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+    <row r="18" spans="1:4" ht="15" customHeight="1"/>
+    <row r="19" spans="1:4" ht="15" customHeight="1"/>
+    <row r="20" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="75">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1201,24 +1219,24 @@
       <c r="C21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+      <c r="D21" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1"/>
+    <row r="23" spans="1:4" ht="15" customHeight="1"/>
+    <row r="24" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A24" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="30.75" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1229,30 +1247,30 @@
         <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
+    <row r="27" spans="1:4" ht="15" customHeight="1"/>
+    <row r="28" spans="1:4" ht="15" customHeight="1"/>
+    <row r="29" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -1262,11 +1280,11 @@
       <c r="C30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D30" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="70.5" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="3" t="s">
         <v>35</v>
@@ -1274,24 +1292,24 @@
       <c r="C31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="D31" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1"/>
+    <row r="33" spans="1:4" ht="15" customHeight="1"/>
+    <row r="34" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A34" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="45">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
@@ -1301,24 +1319,24 @@
       <c r="C35" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="6" t="s">
+      <c r="D35" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1"/>
+    <row r="37" spans="1:4" ht="15" customHeight="1"/>
+    <row r="38" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A38" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="210.75" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>40</v>
       </c>
@@ -1328,24 +1346,24 @@
       <c r="C39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
+      <c r="D39" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1"/>
+    <row r="41" spans="1:4" ht="15" customHeight="1"/>
+    <row r="42" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="60">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -1355,24 +1373,24 @@
       <c r="C43" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="6" t="s">
+      <c r="D43" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1"/>
+    <row r="45" spans="1:4" ht="15" customHeight="1"/>
+    <row r="46" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A46" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="75">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -1382,11 +1400,11 @@
       <c r="C47" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="D47" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="45">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>49</v>
@@ -1394,24 +1412,24 @@
       <c r="C48" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="6" t="s">
+      <c r="D48" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" customHeight="1"/>
+    <row r="50" spans="1:4" ht="15" customHeight="1"/>
+    <row r="51" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A51" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="90">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -1422,23 +1440,23 @@
         <v>53</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" customHeight="1"/>
+    <row r="54" spans="1:4" ht="15" customHeight="1"/>
+    <row r="55" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A55" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" ht="60">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -1449,17 +1467,17 @@
         <v>58</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:4" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="90">
       <c r="A58" s="3" t="s">
         <v>56</v>
       </c>
@@ -1469,38 +1487,38 @@
       <c r="C58" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="6" t="s">
+      <c r="D58" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" customHeight="1"/>
+    <row r="60" spans="1:4" ht="15" customHeight="1"/>
+    <row r="61" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A61" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="75">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="D62" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="45">
       <c r="A63" s="2"/>
       <c r="B63" s="3" t="s">
         <v>64</v>
@@ -1508,24 +1526,24 @@
       <c r="C63" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="66" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="6" t="s">
+      <c r="D63" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" customHeight="1"/>
+    <row r="65" spans="1:4" ht="15" customHeight="1"/>
+    <row r="66" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A66" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" ht="42">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
@@ -1535,24 +1553,24 @@
       <c r="C67" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="6" t="s">
+      <c r="D67" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" customHeight="1"/>
+    <row r="69" spans="1:4" ht="15" customHeight="1"/>
+    <row r="70" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A70" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" ht="45">
       <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
@@ -1563,7 +1581,7 @@
         <v>71</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1582,6 +1600,11 @@
     <hyperlink ref="B2" r:id="rId12" display="http://webaim.org/techniques/alttext/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>